<commit_message>
Atualização dos niveis, e nivel7_h
</commit_message>
<xml_diff>
--- a/status_jogo/inimigos_masmorra.xlsx
+++ b/status_jogo/inimigos_masmorra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUPORTE 03\Desktop\EU\Eu (Carlos)\Cod_Dev\Masmorra_fim\status_jogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1620255-2D27-46BC-A0E4-B7572E4BE655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AF31AC-E881-4F0B-A316-5877FA9ADFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-60" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,6 +474,13 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,7 +794,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,8 +976,8 @@
       <c r="R4" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="S4" s="15" t="s">
-        <v>63</v>
+      <c r="S4" s="14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -1019,8 +1026,8 @@
       <c r="R5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="14" t="s">
-        <v>64</v>
+      <c r="S5" s="15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -1070,7 +1077,7 @@
         <v>58</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -1168,6 +1175,7 @@
       <c r="J9" s="5">
         <v>4</v>
       </c>
+      <c r="S9" s="19"/>
     </row>
     <row r="10" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1200,6 +1208,7 @@
       <c r="J10" s="5">
         <v>4</v>
       </c>
+      <c r="S10" s="20"/>
     </row>
     <row r="11" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1232,6 +1241,7 @@
       <c r="J11" s="5">
         <v>4</v>
       </c>
+      <c r="S11" s="20"/>
     </row>
     <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1264,6 +1274,7 @@
       <c r="J12" s="5">
         <v>4</v>
       </c>
+      <c r="S12" s="21"/>
     </row>
     <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1296,6 +1307,7 @@
       <c r="J13" s="6">
         <v>5</v>
       </c>
+      <c r="S13" s="19"/>
     </row>
     <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">

</xml_diff>